<commit_message>
Alternative setup with SQL files
One SQL file for each exercise. JSON-like parameters for visualization can (only) be embedded into first comment block. Parameters j_fig and j_trace must follow Plotly JSON schema.
</commit_message>
<xml_diff>
--- a/Data Analyst/exercise_results.xlsx
+++ b/Data Analyst/exercise_results.xlsx
@@ -9,6 +9,9 @@
     <sheet name="q2_close_ended" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="q3_close_ended" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="q2_open_ended" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="q2_close_ended.sql" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="q3_close_ended.sql" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="q2_open_ended.sql" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -455,15 +458,15 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>brand</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>total_sales</t>
         </is>
@@ -2790,4 +2793,2353 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>brand</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>total_sales</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>CVS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>DOVE</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>30.91</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>TRIDENT</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>23.36</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>COORS LIGHT</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>17.48</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>TRESEMMÉ</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>14.58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>major_category</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>count_users</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>generation</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>total_sales</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>percent_total_sale</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Health &amp; Wellness</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Baby Boomers</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>84.09</v>
+      </c>
+      <c r="E2" t="n">
+        <v>53.53663971477685</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Health &amp; Wellness</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>7</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Generation X</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>37.81</v>
+      </c>
+      <c r="E3" t="n">
+        <v>24.07206977780608</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Health &amp; Wellness</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Millennials</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>35.17</v>
+      </c>
+      <c r="E4" t="n">
+        <v>22.39129050741708</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J59"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>brand</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>sub_category</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>total_receipts</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>total_sales</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>avg_sales_per_receipt</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>total_qty</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>avg_sales_per_qty</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>total_users</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>users_in_table</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>distinct_users</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>TOSTITOS</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>35</v>
+      </c>
+      <c r="D2" t="n">
+        <v>177.32</v>
+      </c>
+      <c r="E2" t="n">
+        <v>5.066285714285714</v>
+      </c>
+      <c r="F2" t="n">
+        <v>37</v>
+      </c>
+      <c r="G2" t="n">
+        <v>4.792432432432432</v>
+      </c>
+      <c r="H2" t="n">
+        <v>35</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>GOOD FOODS</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Salsa</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>9</v>
+      </c>
+      <c r="D3" t="n">
+        <v>94.91</v>
+      </c>
+      <c r="E3" t="n">
+        <v>10.54555555555556</v>
+      </c>
+      <c r="F3" t="n">
+        <v>9</v>
+      </c>
+      <c r="G3" t="n">
+        <v>10.54555555555556</v>
+      </c>
+      <c r="H3" t="n">
+        <v>9</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>PACE</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Salsa</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>22</v>
+      </c>
+      <c r="D4" t="n">
+        <v>79.73</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3.624090909090909</v>
+      </c>
+      <c r="F4" t="n">
+        <v>22</v>
+      </c>
+      <c r="G4" t="n">
+        <v>3.624090909090909</v>
+      </c>
+      <c r="H4" t="n">
+        <v>22</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>FRITOS</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>18</v>
+      </c>
+      <c r="D5" t="n">
+        <v>63.18</v>
+      </c>
+      <c r="E5" t="n">
+        <v>3.51</v>
+      </c>
+      <c r="F5" t="n">
+        <v>19</v>
+      </c>
+      <c r="G5" t="n">
+        <v>3.325263157894737</v>
+      </c>
+      <c r="H5" t="n">
+        <v>18</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>MARKETSIDE</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>14</v>
+      </c>
+      <c r="D6" t="n">
+        <v>56.3</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4.021428571428571</v>
+      </c>
+      <c r="F6" t="n">
+        <v>14</v>
+      </c>
+      <c r="G6" t="n">
+        <v>4.021428571428571</v>
+      </c>
+      <c r="H6" t="n">
+        <v>14</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>HELUVA GOOD!</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>14</v>
+      </c>
+      <c r="D7" t="n">
+        <v>52.01</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3.715</v>
+      </c>
+      <c r="F7" t="n">
+        <v>14</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3.715</v>
+      </c>
+      <c r="H7" t="n">
+        <v>14</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>MARZETTI</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>11</v>
+      </c>
+      <c r="D8" t="n">
+        <v>51.14</v>
+      </c>
+      <c r="E8" t="n">
+        <v>4.649090909090909</v>
+      </c>
+      <c r="F8" t="n">
+        <v>11</v>
+      </c>
+      <c r="G8" t="n">
+        <v>4.649090909090909</v>
+      </c>
+      <c r="H8" t="n">
+        <v>11</v>
+      </c>
+      <c r="I8" t="n">
+        <v>2</v>
+      </c>
+      <c r="J8" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>FRESHNESS GUARANTEED</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Salsa</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>11</v>
+      </c>
+      <c r="D9" t="n">
+        <v>42.48</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3.861818181818181</v>
+      </c>
+      <c r="F9" t="n">
+        <v>11</v>
+      </c>
+      <c r="G9" t="n">
+        <v>3.861818181818181</v>
+      </c>
+      <c r="H9" t="n">
+        <v>11</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>DEAN'S DAIRY DIP</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>17</v>
+      </c>
+      <c r="D10" t="n">
+        <v>39.95</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="F10" t="n">
+        <v>17</v>
+      </c>
+      <c r="G10" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="H10" t="n">
+        <v>17</v>
+      </c>
+      <c r="I10" t="n">
+        <v>17</v>
+      </c>
+      <c r="J10" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>HIDDEN VALLEY RANCH</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>9</v>
+      </c>
+      <c r="D11" t="n">
+        <v>38.06</v>
+      </c>
+      <c r="E11" t="n">
+        <v>4.228888888888889</v>
+      </c>
+      <c r="F11" t="n">
+        <v>10</v>
+      </c>
+      <c r="G11" t="n">
+        <v>3.806</v>
+      </c>
+      <c r="H11" t="n">
+        <v>9</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>KIRKLAND SIGNATURE</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Salsa</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>3</v>
+      </c>
+      <c r="D12" t="n">
+        <v>37.47</v>
+      </c>
+      <c r="E12" t="n">
+        <v>12.49</v>
+      </c>
+      <c r="F12" t="n">
+        <v>3</v>
+      </c>
+      <c r="G12" t="n">
+        <v>12.49</v>
+      </c>
+      <c r="H12" t="n">
+        <v>3</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>SABRA</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>9</v>
+      </c>
+      <c r="D13" t="n">
+        <v>33.01000000000001</v>
+      </c>
+      <c r="E13" t="n">
+        <v>3.667777777777778</v>
+      </c>
+      <c r="F13" t="n">
+        <v>9</v>
+      </c>
+      <c r="G13" t="n">
+        <v>3.667777777777778</v>
+      </c>
+      <c r="H13" t="n">
+        <v>9</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>HIDDEN VALLEY</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>10</v>
+      </c>
+      <c r="D14" t="n">
+        <v>31.26</v>
+      </c>
+      <c r="E14" t="n">
+        <v>3.126</v>
+      </c>
+      <c r="F14" t="n">
+        <v>16</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1.95375</v>
+      </c>
+      <c r="H14" t="n">
+        <v>10</v>
+      </c>
+      <c r="I14" t="n">
+        <v>10</v>
+      </c>
+      <c r="J14" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>PRIVATE LABEL</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>9</v>
+      </c>
+      <c r="D15" t="n">
+        <v>30.25</v>
+      </c>
+      <c r="E15" t="n">
+        <v>3.361111111111111</v>
+      </c>
+      <c r="F15" t="n">
+        <v>9</v>
+      </c>
+      <c r="G15" t="n">
+        <v>3.361111111111111</v>
+      </c>
+      <c r="H15" t="n">
+        <v>9</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>LAY'S</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>6</v>
+      </c>
+      <c r="D16" t="n">
+        <v>28.92</v>
+      </c>
+      <c r="E16" t="n">
+        <v>4.82</v>
+      </c>
+      <c r="F16" t="n">
+        <v>7</v>
+      </c>
+      <c r="G16" t="n">
+        <v>4.131428571428572</v>
+      </c>
+      <c r="H16" t="n">
+        <v>6</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>MEMBER'S MARK</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>4</v>
+      </c>
+      <c r="D17" t="n">
+        <v>28.92</v>
+      </c>
+      <c r="E17" t="n">
+        <v>7.23</v>
+      </c>
+      <c r="F17" t="n">
+        <v>4</v>
+      </c>
+      <c r="G17" t="n">
+        <v>7.23</v>
+      </c>
+      <c r="H17" t="n">
+        <v>4</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>HERDEZ</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Salsa</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>9</v>
+      </c>
+      <c r="D18" t="n">
+        <v>28.75</v>
+      </c>
+      <c r="E18" t="n">
+        <v>3.194444444444445</v>
+      </c>
+      <c r="F18" t="n">
+        <v>9</v>
+      </c>
+      <c r="G18" t="n">
+        <v>3.194444444444445</v>
+      </c>
+      <c r="H18" t="n">
+        <v>9</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>LITEHOUSE</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>4</v>
+      </c>
+      <c r="D19" t="n">
+        <v>23.44</v>
+      </c>
+      <c r="E19" t="n">
+        <v>5.86</v>
+      </c>
+      <c r="F19" t="n">
+        <v>4</v>
+      </c>
+      <c r="G19" t="n">
+        <v>5.86</v>
+      </c>
+      <c r="H19" t="n">
+        <v>4</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>FRESH CRAVINGS</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>7</v>
+      </c>
+      <c r="D20" t="n">
+        <v>21.51</v>
+      </c>
+      <c r="E20" t="n">
+        <v>3.072857142857143</v>
+      </c>
+      <c r="F20" t="n">
+        <v>7</v>
+      </c>
+      <c r="G20" t="n">
+        <v>3.072857142857143</v>
+      </c>
+      <c r="H20" t="n">
+        <v>7</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>GOOD &amp; GATHER</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>5</v>
+      </c>
+      <c r="D21" t="n">
+        <v>16.75</v>
+      </c>
+      <c r="E21" t="n">
+        <v>3.35</v>
+      </c>
+      <c r="F21" t="n">
+        <v>5</v>
+      </c>
+      <c r="G21" t="n">
+        <v>3.35</v>
+      </c>
+      <c r="H21" t="n">
+        <v>5</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>WHOLLY</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Salsa</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>3</v>
+      </c>
+      <c r="D22" t="n">
+        <v>16.75</v>
+      </c>
+      <c r="E22" t="n">
+        <v>5.583333333333333</v>
+      </c>
+      <c r="F22" t="n">
+        <v>3</v>
+      </c>
+      <c r="G22" t="n">
+        <v>5.583333333333333</v>
+      </c>
+      <c r="H22" t="n">
+        <v>3</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>YUCATAN</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Salsa</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>4</v>
+      </c>
+      <c r="D23" t="n">
+        <v>15.68</v>
+      </c>
+      <c r="E23" t="n">
+        <v>3.92</v>
+      </c>
+      <c r="F23" t="n">
+        <v>4</v>
+      </c>
+      <c r="G23" t="n">
+        <v>3.92</v>
+      </c>
+      <c r="H23" t="n">
+        <v>4</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>GREAT VALUE</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Salsa</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>6</v>
+      </c>
+      <c r="D24" t="n">
+        <v>15</v>
+      </c>
+      <c r="E24" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F24" t="n">
+        <v>8</v>
+      </c>
+      <c r="G24" t="n">
+        <v>1.875</v>
+      </c>
+      <c r="H24" t="n">
+        <v>6</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>MURRAY'S</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>2</v>
+      </c>
+      <c r="D25" t="n">
+        <v>13.04</v>
+      </c>
+      <c r="E25" t="n">
+        <v>6.52</v>
+      </c>
+      <c r="F25" t="n">
+        <v>2</v>
+      </c>
+      <c r="G25" t="n">
+        <v>6.52</v>
+      </c>
+      <c r="H25" t="n">
+        <v>2</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>NUTELLA</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" t="n">
+        <v>12.98</v>
+      </c>
+      <c r="E26" t="n">
+        <v>12.98</v>
+      </c>
+      <c r="F26" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" t="n">
+        <v>12.98</v>
+      </c>
+      <c r="H26" t="n">
+        <v>1</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>MRS WAGES</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>4</v>
+      </c>
+      <c r="D27" t="n">
+        <v>12.88</v>
+      </c>
+      <c r="E27" t="n">
+        <v>3.22</v>
+      </c>
+      <c r="F27" t="n">
+        <v>4</v>
+      </c>
+      <c r="G27" t="n">
+        <v>3.22</v>
+      </c>
+      <c r="H27" t="n">
+        <v>4</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>GORDO'S DIPS</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>3</v>
+      </c>
+      <c r="D28" t="n">
+        <v>9.960000000000001</v>
+      </c>
+      <c r="E28" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="F28" t="n">
+        <v>3</v>
+      </c>
+      <c r="G28" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="H28" t="n">
+        <v>3</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>BOAR'S HEAD</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>2</v>
+      </c>
+      <c r="D29" t="n">
+        <v>9.48</v>
+      </c>
+      <c r="E29" t="n">
+        <v>4.74</v>
+      </c>
+      <c r="F29" t="n">
+        <v>2</v>
+      </c>
+      <c r="G29" t="n">
+        <v>4.74</v>
+      </c>
+      <c r="H29" t="n">
+        <v>2</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>MATEO'S GOURMET SALSA</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Salsa</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>2</v>
+      </c>
+      <c r="D30" t="n">
+        <v>9.34</v>
+      </c>
+      <c r="E30" t="n">
+        <v>4.67</v>
+      </c>
+      <c r="F30" t="n">
+        <v>2</v>
+      </c>
+      <c r="G30" t="n">
+        <v>4.67</v>
+      </c>
+      <c r="H30" t="n">
+        <v>2</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>MEIJER</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>2</v>
+      </c>
+      <c r="D31" t="n">
+        <v>9.18</v>
+      </c>
+      <c r="E31" t="n">
+        <v>4.59</v>
+      </c>
+      <c r="F31" t="n">
+        <v>2</v>
+      </c>
+      <c r="G31" t="n">
+        <v>4.59</v>
+      </c>
+      <c r="H31" t="n">
+        <v>2</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>DEAN'S DAIRY</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>3</v>
+      </c>
+      <c r="D32" t="n">
+        <v>8.67</v>
+      </c>
+      <c r="E32" t="n">
+        <v>2.89</v>
+      </c>
+      <c r="F32" t="n">
+        <v>3</v>
+      </c>
+      <c r="G32" t="n">
+        <v>2.89</v>
+      </c>
+      <c r="H32" t="n">
+        <v>3</v>
+      </c>
+      <c r="I32" t="n">
+        <v>1</v>
+      </c>
+      <c r="J32" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>NEWMAN’S OWN</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Salsa</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>3</v>
+      </c>
+      <c r="D33" t="n">
+        <v>8.48</v>
+      </c>
+      <c r="E33" t="n">
+        <v>2.826666666666667</v>
+      </c>
+      <c r="F33" t="n">
+        <v>3</v>
+      </c>
+      <c r="G33" t="n">
+        <v>2.826666666666667</v>
+      </c>
+      <c r="H33" t="n">
+        <v>3</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>ON THE BORDER SNACKS</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>2</v>
+      </c>
+      <c r="D34" t="n">
+        <v>7.49</v>
+      </c>
+      <c r="E34" t="n">
+        <v>3.745</v>
+      </c>
+      <c r="F34" t="n">
+        <v>2</v>
+      </c>
+      <c r="G34" t="n">
+        <v>3.745</v>
+      </c>
+      <c r="H34" t="n">
+        <v>2</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>PRIVATE SELECTION</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Salsa</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>2</v>
+      </c>
+      <c r="D35" t="n">
+        <v>6.78</v>
+      </c>
+      <c r="E35" t="n">
+        <v>3.39</v>
+      </c>
+      <c r="F35" t="n">
+        <v>2</v>
+      </c>
+      <c r="G35" t="n">
+        <v>3.39</v>
+      </c>
+      <c r="H35" t="n">
+        <v>2</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>TACO BELL GROCERY</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>2</v>
+      </c>
+      <c r="D36" t="n">
+        <v>6.45</v>
+      </c>
+      <c r="E36" t="n">
+        <v>3.225</v>
+      </c>
+      <c r="F36" t="n">
+        <v>2</v>
+      </c>
+      <c r="G36" t="n">
+        <v>3.225</v>
+      </c>
+      <c r="H36" t="n">
+        <v>2</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>JULIOS</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" t="n">
+        <v>5.98</v>
+      </c>
+      <c r="E37" t="n">
+        <v>5.98</v>
+      </c>
+      <c r="F37" t="n">
+        <v>1</v>
+      </c>
+      <c r="G37" t="n">
+        <v>5.98</v>
+      </c>
+      <c r="H37" t="n">
+        <v>1</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>DAISY</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" t="n">
+        <v>5.58</v>
+      </c>
+      <c r="E38" t="n">
+        <v>5.58</v>
+      </c>
+      <c r="F38" t="n">
+        <v>2</v>
+      </c>
+      <c r="G38" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="H38" t="n">
+        <v>1</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>LA TERRA FINA</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" t="n">
+        <v>5.49</v>
+      </c>
+      <c r="E39" t="n">
+        <v>5.49</v>
+      </c>
+      <c r="F39" t="n">
+        <v>1</v>
+      </c>
+      <c r="G39" t="n">
+        <v>5.49</v>
+      </c>
+      <c r="H39" t="n">
+        <v>1</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>SIGNATURE SELECT</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Salsa</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>1</v>
+      </c>
+      <c r="D40" t="n">
+        <v>5.49</v>
+      </c>
+      <c r="E40" t="n">
+        <v>5.49</v>
+      </c>
+      <c r="F40" t="n">
+        <v>1</v>
+      </c>
+      <c r="G40" t="n">
+        <v>5.49</v>
+      </c>
+      <c r="H40" t="n">
+        <v>1</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>WELLSLEY FARMS</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Salsa</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" t="n">
+        <v>5.49</v>
+      </c>
+      <c r="E41" t="n">
+        <v>5.49</v>
+      </c>
+      <c r="F41" t="n">
+        <v>1</v>
+      </c>
+      <c r="G41" t="n">
+        <v>5.49</v>
+      </c>
+      <c r="H41" t="n">
+        <v>1</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>FODY</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Salsa</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>1</v>
+      </c>
+      <c r="D42" t="n">
+        <v>5.48</v>
+      </c>
+      <c r="E42" t="n">
+        <v>5.48</v>
+      </c>
+      <c r="F42" t="n">
+        <v>1</v>
+      </c>
+      <c r="G42" t="n">
+        <v>5.48</v>
+      </c>
+      <c r="H42" t="n">
+        <v>1</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>PRAIRIE FARMS</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>3</v>
+      </c>
+      <c r="D43" t="n">
+        <v>5.34</v>
+      </c>
+      <c r="E43" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="F43" t="n">
+        <v>3</v>
+      </c>
+      <c r="G43" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="H43" t="n">
+        <v>3</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>TASTE OF THE SOUTH</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>1</v>
+      </c>
+      <c r="D44" t="n">
+        <v>4.98</v>
+      </c>
+      <c r="E44" t="n">
+        <v>4.98</v>
+      </c>
+      <c r="F44" t="n">
+        <v>1</v>
+      </c>
+      <c r="G44" t="n">
+        <v>4.98</v>
+      </c>
+      <c r="H44" t="n">
+        <v>1</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>ESTI</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>1</v>
+      </c>
+      <c r="D45" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="E45" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="F45" t="n">
+        <v>1</v>
+      </c>
+      <c r="G45" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="H45" t="n">
+        <v>1</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>CLINTS</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Salsa</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>1</v>
+      </c>
+      <c r="D46" t="n">
+        <v>3.97</v>
+      </c>
+      <c r="E46" t="n">
+        <v>3.97</v>
+      </c>
+      <c r="F46" t="n">
+        <v>1</v>
+      </c>
+      <c r="G46" t="n">
+        <v>3.97</v>
+      </c>
+      <c r="H46" t="n">
+        <v>1</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>FRESH CREATIONS</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>1</v>
+      </c>
+      <c r="D47" t="n">
+        <v>3.69</v>
+      </c>
+      <c r="E47" t="n">
+        <v>3.69</v>
+      </c>
+      <c r="F47" t="n">
+        <v>1</v>
+      </c>
+      <c r="G47" t="n">
+        <v>3.69</v>
+      </c>
+      <c r="H47" t="n">
+        <v>1</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>O ORGANICS</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Salsa</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>1</v>
+      </c>
+      <c r="D48" t="n">
+        <v>3.59</v>
+      </c>
+      <c r="E48" t="n">
+        <v>3.59</v>
+      </c>
+      <c r="F48" t="n">
+        <v>1</v>
+      </c>
+      <c r="G48" t="n">
+        <v>3.59</v>
+      </c>
+      <c r="H48" t="n">
+        <v>1</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>CHI-CHI'S</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Salsa</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>2</v>
+      </c>
+      <c r="D49" t="n">
+        <v>3.57</v>
+      </c>
+      <c r="E49" t="n">
+        <v>1.785</v>
+      </c>
+      <c r="F49" t="n">
+        <v>2</v>
+      </c>
+      <c r="G49" t="n">
+        <v>1.785</v>
+      </c>
+      <c r="H49" t="n">
+        <v>2</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>FRITO-LAY</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>1</v>
+      </c>
+      <c r="D50" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E50" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="F50" t="n">
+        <v>1</v>
+      </c>
+      <c r="G50" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="H50" t="n">
+        <v>1</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>BISON</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>1</v>
+      </c>
+      <c r="D51" t="n">
+        <v>3.29</v>
+      </c>
+      <c r="E51" t="n">
+        <v>3.29</v>
+      </c>
+      <c r="F51" t="n">
+        <v>1</v>
+      </c>
+      <c r="G51" t="n">
+        <v>3.29</v>
+      </c>
+      <c r="H51" t="n">
+        <v>1</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J51" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>MISSION</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Salsa</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>1</v>
+      </c>
+      <c r="D52" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="E52" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="F52" t="n">
+        <v>1</v>
+      </c>
+      <c r="G52" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="H52" t="n">
+        <v>1</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0</v>
+      </c>
+      <c r="J52" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>HILAND</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>2</v>
+      </c>
+      <c r="D53" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="E53" t="n">
+        <v>1.625</v>
+      </c>
+      <c r="F53" t="n">
+        <v>2</v>
+      </c>
+      <c r="G53" t="n">
+        <v>1.625</v>
+      </c>
+      <c r="H53" t="n">
+        <v>2</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>CREAMLAND DAIRY</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>1</v>
+      </c>
+      <c r="D54" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="E54" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="F54" t="n">
+        <v>1</v>
+      </c>
+      <c r="G54" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="H54" t="n">
+        <v>1</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0</v>
+      </c>
+      <c r="J54" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>LA PREFERIDA</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>1</v>
+      </c>
+      <c r="D55" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="E55" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="F55" t="n">
+        <v>1</v>
+      </c>
+      <c r="G55" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="H55" t="n">
+        <v>1</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0</v>
+      </c>
+      <c r="J55" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>ALWAYS SAVE</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Salsa</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>1</v>
+      </c>
+      <c r="D56" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="E56" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="F56" t="n">
+        <v>1</v>
+      </c>
+      <c r="G56" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="H56" t="n">
+        <v>1</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>ISADORA</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>1</v>
+      </c>
+      <c r="D57" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="E57" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="F57" t="n">
+        <v>1</v>
+      </c>
+      <c r="G57" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="H57" t="n">
+        <v>1</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0</v>
+      </c>
+      <c r="J57" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>UTZ</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>1</v>
+      </c>
+      <c r="D58" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="E58" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="F58" t="n">
+        <v>1</v>
+      </c>
+      <c r="G58" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="H58" t="n">
+        <v>1</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>ZACCA</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Dips</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>1</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0</v>
+      </c>
+      <c r="F59" t="n">
+        <v>1</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0</v>
+      </c>
+      <c r="H59" t="n">
+        <v>1</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0</v>
+      </c>
+      <c r="J59" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>